<commit_message>
Updated jxls 2 report in demo db
</commit_message>
<xml_diff>
--- a/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls2.xlsx
+++ b/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls2.xlsx
@@ -15,8 +15,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="E10")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="results" var="row" lastCell="E10")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Sample jxls report</t>
   </si>
@@ -27,15 +85,6 @@
     <t>Data:</t>
   </si>
   <si>
-    <t>${order_date}</t>
-  </si>
-  <si>
-    <t>City: ${city}</t>
-  </si>
-  <si>
-    <t>Items: ${item}</t>
-  </si>
-  <si>
     <t>Order ID</t>
   </si>
   <si>
@@ -48,32 +97,45 @@
     <t>Volume</t>
   </si>
   <si>
-    <t>${results.ORDER_ID}</t>
-  </si>
-  <si>
-    <t>${results.CITY_NAME}</t>
-  </si>
-  <si>
-    <t>${results.ORDER_DATE}</t>
-  </si>
-  <si>
-    <t>${results.VOLUME}</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
-    <t>${results.ITEM_NAME}</t>
+    <t>${row.ORDER_ID}</t>
+  </si>
+  <si>
+    <t>${row.CITY_NAME}</t>
+  </si>
+  <si>
+    <t>${row.ITEM_NAME}</t>
+  </si>
+  <si>
+    <t>${row.ORDER_DATE}</t>
+  </si>
+  <si>
+    <t>${row.VOLUME}</t>
+  </si>
+  <si>
+    <t>${order_date.value}</t>
+  </si>
+  <si>
+    <t>${cityId.parameter.label}</t>
+  </si>
+  <si>
+    <t>${cityId.value}</t>
+  </si>
+  <si>
+    <t>${item.nameAndDisplayValues}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +171,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -136,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -146,6 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,15 +522,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,18 +548,21 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
+      <c r="A4" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -490,36 +572,36 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -529,6 +611,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated some demo reports
</commit_message>
<xml_diff>
--- a/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls2.xlsx
+++ b/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls2.xlsx
@@ -100,21 +100,6 @@
     <t>Item</t>
   </si>
   <si>
-    <t>${row.ORDER_ID}</t>
-  </si>
-  <si>
-    <t>${row.CITY_NAME}</t>
-  </si>
-  <si>
-    <t>${row.ITEM_NAME}</t>
-  </si>
-  <si>
-    <t>${row.ORDER_DATE}</t>
-  </si>
-  <si>
-    <t>${row.VOLUME}</t>
-  </si>
-  <si>
     <t>${order_date.value}</t>
   </si>
   <si>
@@ -125,6 +110,21 @@
   </si>
   <si>
     <t>${item.labelAndDisplayValues}</t>
+  </si>
+  <si>
+    <t>${row.order_id}</t>
+  </si>
+  <si>
+    <t>${row.city_name}</t>
+  </si>
+  <si>
+    <t>${row.item_name}</t>
+  </si>
+  <si>
+    <t>${row.order_date}</t>
+  </si>
+  <si>
+    <t>${row.volume}</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,20 +549,20 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -589,19 +589,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1"/>
     </row>

</xml_diff>